<commit_message>
modified:   app/data/RaceRoutes.xlsx 	modified:   app/heuristics/loop/__pycache__/loop.cpython-36.pyc 	modified:   app/heuristics/loop/loop.py 	modified:   app/run.py
</commit_message>
<xml_diff>
--- a/app/data/RaceRoutes.xlsx
+++ b/app/data/RaceRoutes.xlsx
@@ -189,7 +189,7 @@
     <t>7 Audubon Gate, Miller Place, NY, US 11764</t>
   </si>
   <si>
-    <t> Christine Camardella</t>
+    <t>Christine Camardella</t>
   </si>
   <si>
     <t> 54 Prentice Road, Levittown, NY US 11756</t>
@@ -252,7 +252,7 @@
     <t>James Hayward</t>
   </si>
   <si>
-    <t> Sue Lawlor</t>
+    <t>Sue Lawlor</t>
   </si>
   <si>
     <t>290 Western Ave. Morristown, NJ US 07960</t>
@@ -1331,7 +1331,7 @@
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="1">
@@ -1859,7 +1859,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B26" s="1">

</xml_diff>

<commit_message>
modified:   app/data/RaceRoutes.xlsx 	modified:   app/heuristics/loop/__pycache__/loop.cpython-36.pyc 	modified:   app/heuristics/loop/loop.py 	modified:   app/routes.zip 	new file:   app/routes/Hayes-route-1.gpx 	new file:   app/routes/Hayes-route-2.gpx 	new file:   app/routes/Hayes-route-3.gpx 	new file:   app/routes/Hayes-route-4.gpx 	new file:   app/routes/Helmer-route-1.gpx 	new file:   app/routes/Helmer-route-2.gpx 	new file:   app/routes/Helmer-route-3.gpx 	new file:   app/routes/JC-route-1.gpx 	new file:   app/routes/JC-route-2.gpx 	new file:   app/routes/JC-route-3.gpx 	new file:   app/routes/JC-route-4.gpx 	new file:   app/routes/O'Connor-route-1.gpx 	new file:   app/routes/O'Connor-route-2.gpx 	new file:   app/routes/O'Connor-route-3.gpx 	new file:   app/routes/O'Connor-route-4.gpx 	modified:   app/run.py
</commit_message>
<xml_diff>
--- a/app/data/RaceRoutes.xlsx
+++ b/app/data/RaceRoutes.xlsx
@@ -4,19 +4,20 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhVmA+m+5k6fvoTwSTEgP0bmmlyVA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhS2rQB/AYaJZnfO3GtPtVerBVL2A=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -45,13 +46,16 @@
     <t>Distance (km)</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>O'Connor</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
   <si>
     <t>Route Buddy?</t>
@@ -72,6 +76,9 @@
     <t>Jeffrey Cergol</t>
   </si>
   <si>
+    <t>Hayes</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
@@ -79,6 +86,12 @@
   </si>
   <si>
     <t>Full</t>
+  </si>
+  <si>
+    <t>Helmer</t>
+  </si>
+  <si>
+    <t>JC</t>
   </si>
   <si>
     <t>20 Carlisle Road, Miller Place, NY</t>
@@ -265,13 +278,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,16 +304,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="16" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="16" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -306,6 +326,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -560,60 +584,60 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
         <v>21.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>2001.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="3">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5">
         <v>43955.0</v>
       </c>
       <c r="I2" s="2">
         <v>5.0</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K2" s="4">
         <v>40.95199</v>
@@ -622,16 +646,16 @@
         <v>-72.99736</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="1">
         <v>1.0</v>
@@ -641,34 +665,34 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>53.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1">
         <v>2002.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3">
+        <v>22</v>
+      </c>
+      <c r="H3" s="5">
         <v>43955.0</v>
       </c>
       <c r="I3" s="2">
         <v>10.0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K3" s="2">
         <v>40.95199</v>
@@ -677,16 +701,16 @@
         <v>-72.99736</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="P3" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="1">
         <v>1.0</v>
@@ -696,34 +720,34 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1">
         <v>22.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1">
         <v>2003.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3">
+        <v>22</v>
+      </c>
+      <c r="H4" s="5">
         <v>43955.0</v>
       </c>
       <c r="I4" s="2">
         <v>5.0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K4" s="2">
         <v>40.95199</v>
@@ -732,16 +756,16 @@
         <v>-72.99736</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="1">
         <v>1.0</v>
@@ -749,34 +773,34 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
         <v>53.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1">
         <v>2004.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="3">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5">
         <v>43955.0</v>
       </c>
       <c r="I5" s="2">
         <v>5.0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K5" s="2">
         <v>40.82405</v>
@@ -785,16 +809,16 @@
         <v>-73.0715</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q5" s="1">
         <v>1.0</v>
@@ -802,34 +826,34 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1">
         <v>54.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1">
         <v>2005.0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="3">
+        <v>22</v>
+      </c>
+      <c r="H6" s="5">
         <v>43955.0</v>
       </c>
       <c r="I6" s="2">
         <v>5.0</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K6" s="2">
         <v>40.96238</v>
@@ -838,16 +862,16 @@
         <v>-73.11282</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="1">
         <v>1.0</v>
@@ -855,34 +879,34 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1">
         <v>54.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
         <v>2006.0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5">
         <v>43955.0</v>
       </c>
       <c r="I7" s="2">
         <v>5.0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K7" s="2">
         <v>40.96238</v>
@@ -891,16 +915,16 @@
         <v>-73.11282</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q7" s="1">
         <v>1.0</v>
@@ -908,34 +932,34 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1">
         <v>14.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1">
         <v>2007.0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="3">
+        <v>22</v>
+      </c>
+      <c r="H8" s="5">
         <v>43955.0</v>
       </c>
       <c r="I8" s="2">
         <v>5.0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K8" s="2">
         <v>40.96238</v>
@@ -944,16 +968,16 @@
         <v>-73.11282</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q8" s="1">
         <v>1.0</v>
@@ -961,34 +985,34 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1">
         <v>11.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1">
         <v>2008.0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="3">
+        <v>22</v>
+      </c>
+      <c r="H9" s="5">
         <v>43955.0</v>
       </c>
       <c r="I9" s="2">
         <v>5.0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="K9" s="2">
         <v>40.96238</v>
@@ -997,16 +1021,16 @@
         <v>-73.11282</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q9" s="1">
         <v>1.0</v>
@@ -1014,34 +1038,34 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1">
         <v>34.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1">
         <v>2009.0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="3">
+        <v>45</v>
+      </c>
+      <c r="H10" s="5">
         <v>43957.0</v>
       </c>
       <c r="I10" s="2">
         <v>5.0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K10" s="2">
         <v>35.32853</v>
@@ -1050,51 +1074,51 @@
         <v>-79.0594</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1">
         <v>24.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1">
         <v>2010.0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="3">
+        <v>22</v>
+      </c>
+      <c r="H11" s="5">
         <v>43957.0</v>
       </c>
       <c r="I11" s="2">
         <v>5.0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K11" s="2">
         <v>35.996201</v>
@@ -1103,16 +1127,16 @@
         <v>-78.910782</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="1">
         <v>2.0</v>
@@ -1120,34 +1144,34 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1">
         <v>16.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1">
         <v>2011.0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="3">
+        <v>22</v>
+      </c>
+      <c r="H12" s="5">
         <v>43957.0</v>
       </c>
       <c r="I12" s="2">
         <v>5.0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="K12" s="2">
         <v>40.94257</v>
@@ -1156,16 +1180,16 @@
         <v>-72.97153</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q12" s="1">
         <v>1.0</v>
@@ -1173,34 +1197,34 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1">
         <v>17.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1">
         <v>2012.0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="3">
+        <v>22</v>
+      </c>
+      <c r="H13" s="5">
         <v>43957.0</v>
       </c>
       <c r="I13" s="2">
         <v>5.0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="K13" s="2">
         <v>40.94257</v>
@@ -1209,16 +1233,16 @@
         <v>-72.97153</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q13" s="1">
         <v>1.0</v>
@@ -1226,34 +1250,34 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1">
         <v>21.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1">
         <v>2013.0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="3">
+        <v>22</v>
+      </c>
+      <c r="H14" s="5">
         <v>43958.0</v>
       </c>
       <c r="I14" s="2">
         <v>5.0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K14" s="2">
         <v>40.93575</v>
@@ -1262,16 +1286,16 @@
         <v>-72.97937</v>
       </c>
       <c r="M14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="P14" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q14" s="1">
         <v>1.0</v>
@@ -1279,34 +1303,34 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1">
         <v>25.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1">
         <v>2014.0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="3">
+        <v>45</v>
+      </c>
+      <c r="H15" s="5">
         <v>43958.0</v>
       </c>
       <c r="I15" s="2">
         <v>5.0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="K15" s="2">
         <v>40.95807</v>
@@ -1315,51 +1339,51 @@
         <v>-73.01179</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1">
         <v>51.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1">
         <v>2015.0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="3">
+        <v>22</v>
+      </c>
+      <c r="H16" s="5">
         <v>43959.0</v>
       </c>
       <c r="I16" s="2">
         <v>10.0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="K16" s="2">
         <v>40.73966</v>
@@ -1368,49 +1392,49 @@
         <v>-73.50534</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="Q16" s="1"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1">
         <v>25.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1">
         <v>2016.0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" s="3">
+        <v>45</v>
+      </c>
+      <c r="H17" s="5">
         <v>43960.0</v>
       </c>
       <c r="I17" s="2">
         <v>10.0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K17" s="2">
         <v>35.996201</v>
@@ -1419,51 +1443,51 @@
         <v>-78.910782</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1">
         <v>28.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1">
         <v>2017.0</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="3">
+        <v>45</v>
+      </c>
+      <c r="H18" s="5">
         <v>43962.0</v>
       </c>
       <c r="I18" s="2">
         <v>5.0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K18" s="2">
         <v>35.32853</v>
@@ -1472,51 +1496,51 @@
         <v>-79.0594</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1">
         <v>64.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1">
         <v>2018.0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="3">
+        <v>45</v>
+      </c>
+      <c r="H19" s="5">
         <v>43964.0</v>
       </c>
       <c r="I19" s="2">
         <v>5.0</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="K19" s="2">
         <v>45.43527</v>
@@ -1525,51 +1549,51 @@
         <v>-122.7949</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1">
         <v>62.0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D20" s="1">
         <v>2019.0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="3">
+        <v>45</v>
+      </c>
+      <c r="H20" s="5">
         <v>43964.0</v>
       </c>
       <c r="I20" s="2">
         <v>10.0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K20" s="2">
         <v>40.70479</v>
@@ -1578,51 +1602,51 @@
         <v>-73.83441</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B21" s="1">
         <v>63.0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1">
         <v>2020.0</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="3">
+        <v>45</v>
+      </c>
+      <c r="H21" s="5">
         <v>43964.0</v>
       </c>
       <c r="I21" s="2">
         <v>10.0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="K21" s="2">
         <v>35.8483</v>
@@ -1631,51 +1655,51 @@
         <v>-86.45946</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1">
         <v>74.0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1">
         <v>2021.0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H22" s="3">
+        <v>45</v>
+      </c>
+      <c r="H22" s="5">
         <v>43964.0</v>
       </c>
       <c r="I22" s="2">
         <v>10.0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="K22" s="2">
         <v>33.95946</v>
@@ -1684,51 +1708,51 @@
         <v>-84.4202</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1">
         <v>42.0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1">
         <v>2022.0</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="3">
+        <v>22</v>
+      </c>
+      <c r="H23" s="5">
         <v>43964.0</v>
       </c>
       <c r="I23" s="2">
         <v>5.0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K23" s="2">
         <v>34.23287</v>
@@ -1737,16 +1761,16 @@
         <v>-118.46265</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="Q23" s="1">
         <v>999.0</v>
@@ -1754,34 +1778,34 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1">
         <v>26.0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1">
         <v>2023.0</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H24" s="3">
+        <v>45</v>
+      </c>
+      <c r="H24" s="5">
         <v>43965.0</v>
       </c>
       <c r="I24" s="2">
         <v>10.0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K24" s="2">
         <v>35.996201</v>
@@ -1790,51 +1814,51 @@
         <v>-78.910782</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1">
         <v>26.0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1">
         <v>2024.0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H25" s="3">
+        <v>45</v>
+      </c>
+      <c r="H25" s="5">
         <v>43965.0</v>
       </c>
       <c r="I25" s="2">
         <v>10.0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K25" s="2">
         <v>35.996201</v>
@@ -1843,51 +1867,51 @@
         <v>-78.910782</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B26" s="1">
         <v>51.0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D26" s="1">
         <v>2025.0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="3">
+        <v>22</v>
+      </c>
+      <c r="H26" s="5">
         <v>43966.0</v>
       </c>
       <c r="I26" s="2">
         <v>10.0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="K26" s="2">
         <v>40.78418</v>
@@ -1896,16 +1920,16 @@
         <v>-74.50322</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="Q26" s="1"/>
     </row>
@@ -13639,4 +13663,149 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>40.94704</v>
+      </c>
+      <c r="D2" s="3">
+        <v>-72.97301</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>40.83808</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-73.00972</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>36.00865</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-79.86963</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>40.95124</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-72.96262</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="36">
+      <c r="D36" s="2"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>